<commit_message>
case2 no multi thread heuristic
</commit_message>
<xml_diff>
--- a/Case2/result.xlsx
+++ b/Case2/result.xlsx
@@ -423,7 +423,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>1.555065870285034</v>
+        <v>1.324806928634644</v>
       </c>
       <c r="C2">
         <v>1308750057.242312</v>
@@ -437,7 +437,7 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>1.504003047943115</v>
+        <v>1.238573789596558</v>
       </c>
       <c r="C3">
         <v>177023302.4490232</v>
@@ -451,7 +451,7 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>5.739963293075562</v>
+        <v>4.952423810958862</v>
       </c>
       <c r="C4">
         <v>583411445.5491903</v>
@@ -465,7 +465,7 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>5.849556922912598</v>
+        <v>5.056061983108521</v>
       </c>
       <c r="C5">
         <v>990347203.3452796</v>
@@ -479,7 +479,7 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>7.076969861984253</v>
+        <v>5.972718954086304</v>
       </c>
       <c r="C6">
         <v>1165435875.946776</v>

</xml_diff>